<commit_message>
updated to print response codes
</commit_message>
<xml_diff>
--- a/files/MAIN_2023-12-26.xlsx
+++ b/files/MAIN_2023-12-26.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\python_stuff\automailer\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124A66AD-1E24-4FE1-A411-2430661BBD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2071,8 +2077,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2148,13 +2154,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2192,7 +2206,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2226,6 +2240,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2260,9 +2275,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2435,14 +2451,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2480,7 +2504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3716933612</v>
       </c>
@@ -2518,7 +2542,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3786883030</v>
       </c>
@@ -2550,7 +2574,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3790092207</v>
       </c>
@@ -2585,7 +2609,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3757235292</v>
       </c>
@@ -2623,7 +2647,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3729120053</v>
       </c>
@@ -2661,7 +2685,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3791812116</v>
       </c>
@@ -2696,7 +2720,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3775716634</v>
       </c>
@@ -2734,7 +2758,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3773645758</v>
       </c>
@@ -2772,7 +2796,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3774939289</v>
       </c>
@@ -2807,7 +2831,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3780122428</v>
       </c>
@@ -2845,7 +2869,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3764392364</v>
       </c>
@@ -2886,7 +2910,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3780053985</v>
       </c>
@@ -2924,7 +2948,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>3743191856</v>
       </c>
@@ -2956,7 +2980,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3778972020</v>
       </c>
@@ -2991,7 +3015,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3703618257</v>
       </c>
@@ -3029,7 +3053,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3575090531</v>
       </c>
@@ -3061,7 +3085,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>3775163984</v>
       </c>
@@ -3093,7 +3117,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3774450037</v>
       </c>
@@ -3131,7 +3155,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3693533935</v>
       </c>
@@ -3166,7 +3190,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3693534895</v>
       </c>
@@ -3201,7 +3225,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3693536674</v>
       </c>
@@ -3236,7 +3260,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3767577724</v>
       </c>
@@ -3271,7 +3295,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>3774458964</v>
       </c>
@@ -3309,7 +3333,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>3774216698</v>
       </c>
@@ -3338,7 +3362,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>3778897611</v>
       </c>
@@ -3379,7 +3403,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3779110996</v>
       </c>
@@ -3417,7 +3441,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3785249512</v>
       </c>
@@ -3452,7 +3476,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>3791523331</v>
       </c>
@@ -3490,7 +3514,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>3779862000</v>
       </c>
@@ -3522,7 +3546,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>3772981858</v>
       </c>
@@ -3560,7 +3584,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>3789954309</v>
       </c>
@@ -3598,7 +3622,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3736477356</v>
       </c>
@@ -3633,7 +3657,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>3772507899</v>
       </c>
@@ -3671,7 +3695,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>3759166127</v>
       </c>
@@ -3703,7 +3727,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>3779912264</v>
       </c>
@@ -3741,7 +3765,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>3785250334</v>
       </c>
@@ -3773,7 +3797,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3616637587</v>
       </c>
@@ -3814,7 +3838,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>3779064039</v>
       </c>
@@ -3852,7 +3876,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>3781553636</v>
       </c>
@@ -3893,7 +3917,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>3641015353</v>
       </c>
@@ -3931,7 +3955,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>3727820700</v>
       </c>
@@ -3972,7 +3996,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>3684120093</v>
       </c>
@@ -4013,7 +4037,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>3792429156</v>
       </c>
@@ -4048,7 +4072,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>3775405705</v>
       </c>
@@ -4083,7 +4107,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>3721375973</v>
       </c>
@@ -4124,7 +4148,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>3777454584</v>
       </c>
@@ -4165,7 +4189,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>3783416267</v>
       </c>
@@ -4203,7 +4227,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>3727428385</v>
       </c>
@@ -4244,7 +4268,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>3725015864</v>
       </c>
@@ -4279,7 +4303,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>3616269964</v>
       </c>
@@ -4317,7 +4341,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>3790491475</v>
       </c>
@@ -4352,7 +4376,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>3775365168</v>
       </c>
@@ -4387,7 +4411,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>3785005424</v>
       </c>
@@ -4425,7 +4449,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>3677794345</v>
       </c>
@@ -4463,7 +4487,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>3783626590</v>
       </c>
@@ -4501,7 +4525,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>3790923638</v>
       </c>
@@ -4536,7 +4560,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>3747544708</v>
       </c>
@@ -4574,7 +4598,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>3765837868</v>
       </c>
@@ -4612,7 +4636,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>3761384366</v>
       </c>
@@ -4650,7 +4674,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>3587841044</v>
       </c>
@@ -4682,7 +4706,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>3731038493</v>
       </c>
@@ -4717,7 +4741,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>3738898017</v>
       </c>
@@ -4752,7 +4776,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>3789263548</v>
       </c>
@@ -4790,7 +4814,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>12</v>
       </c>
@@ -4828,7 +4852,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>13</v>
       </c>
@@ -4866,7 +4890,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>14</v>
       </c>
@@ -4901,7 +4925,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>15</v>
       </c>
@@ -4939,7 +4963,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>16</v>
       </c>
@@ -4979,74 +5003,74 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
-    <hyperlink ref="M4" r:id="rId3"/>
-    <hyperlink ref="M5" r:id="rId4"/>
-    <hyperlink ref="M6" r:id="rId5"/>
-    <hyperlink ref="M7" r:id="rId6"/>
-    <hyperlink ref="M8" r:id="rId7"/>
-    <hyperlink ref="M9" r:id="rId8"/>
-    <hyperlink ref="M10" r:id="rId9"/>
-    <hyperlink ref="M11" r:id="rId10"/>
-    <hyperlink ref="M12" r:id="rId11"/>
-    <hyperlink ref="M13" r:id="rId12"/>
-    <hyperlink ref="M14" r:id="rId13"/>
-    <hyperlink ref="M15" r:id="rId14"/>
-    <hyperlink ref="M16" r:id="rId15"/>
-    <hyperlink ref="M17" r:id="rId16"/>
-    <hyperlink ref="M18" r:id="rId17"/>
-    <hyperlink ref="M19" r:id="rId18"/>
-    <hyperlink ref="M20" r:id="rId19"/>
-    <hyperlink ref="M21" r:id="rId20"/>
-    <hyperlink ref="M22" r:id="rId21"/>
-    <hyperlink ref="M23" r:id="rId22"/>
-    <hyperlink ref="M24" r:id="rId23"/>
-    <hyperlink ref="M25" r:id="rId24"/>
-    <hyperlink ref="M26" r:id="rId25"/>
-    <hyperlink ref="M27" r:id="rId26"/>
-    <hyperlink ref="M28" r:id="rId27"/>
-    <hyperlink ref="M29" r:id="rId28"/>
-    <hyperlink ref="M30" r:id="rId29"/>
-    <hyperlink ref="M31" r:id="rId30"/>
-    <hyperlink ref="M32" r:id="rId31"/>
-    <hyperlink ref="M33" r:id="rId32"/>
-    <hyperlink ref="M34" r:id="rId33"/>
-    <hyperlink ref="M35" r:id="rId34"/>
-    <hyperlink ref="M36" r:id="rId35"/>
-    <hyperlink ref="M37" r:id="rId36"/>
-    <hyperlink ref="M38" r:id="rId37"/>
-    <hyperlink ref="M39" r:id="rId38"/>
-    <hyperlink ref="M40" r:id="rId39"/>
-    <hyperlink ref="M41" r:id="rId40"/>
-    <hyperlink ref="M42" r:id="rId41"/>
-    <hyperlink ref="M43" r:id="rId42"/>
-    <hyperlink ref="M44" r:id="rId43"/>
-    <hyperlink ref="M45" r:id="rId44"/>
-    <hyperlink ref="M46" r:id="rId45"/>
-    <hyperlink ref="M47" r:id="rId46"/>
-    <hyperlink ref="M48" r:id="rId47"/>
-    <hyperlink ref="M49" r:id="rId48"/>
-    <hyperlink ref="M50" r:id="rId49"/>
-    <hyperlink ref="M51" r:id="rId50"/>
-    <hyperlink ref="M52" r:id="rId51"/>
-    <hyperlink ref="M53" r:id="rId52"/>
-    <hyperlink ref="M54" r:id="rId53"/>
-    <hyperlink ref="M55" r:id="rId54"/>
-    <hyperlink ref="M56" r:id="rId55"/>
-    <hyperlink ref="M57" r:id="rId56"/>
-    <hyperlink ref="M58" r:id="rId57"/>
-    <hyperlink ref="M59" r:id="rId58"/>
-    <hyperlink ref="M60" r:id="rId59"/>
-    <hyperlink ref="M61" r:id="rId60"/>
-    <hyperlink ref="M62" r:id="rId61"/>
-    <hyperlink ref="M63" r:id="rId62"/>
-    <hyperlink ref="M64" r:id="rId63"/>
-    <hyperlink ref="M65" r:id="rId64"/>
-    <hyperlink ref="M66" r:id="rId65"/>
-    <hyperlink ref="M67" r:id="rId66"/>
-    <hyperlink ref="M68" r:id="rId67"/>
-    <hyperlink ref="M69" r:id="rId68"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="M6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="M7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="M8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="M9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="M10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="M11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="M12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="M13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="M14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="M15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="M16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="M17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="M18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="M19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="M20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="M21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="M22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="M23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="M24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="M25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="M26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="M27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="M28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="M29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="M30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="M31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="M32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="M33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="M34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="M35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="M36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="M37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="M38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="M39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="M40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="M41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="M42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="M43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="M44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="M45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="M46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="M47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="M48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="M49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="M50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="M51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="M52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="M53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="M54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="M55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="M56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="M57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="M58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="M59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="M60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="M61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="M62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="M63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="M64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="M65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="M66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="M67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="M68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="M69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>